<commit_message>
update code, test, fix errors when closing door, fix req_door_open in gui.fl
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh\Desktop\spring 2025\Fundamental\FUNDAMENTAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh\Desktop\spring 2025\Fundamental\FUNDAMENTAL\elevatorSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D646A578-2FC3-4F74-829E-6BAA6537CA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2591E803-757F-49CD-AF6F-C94CCF769301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F06D82AD-8A9D-49AA-9081-ABD8D37343FA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="120">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -49,9 +49,6 @@
     <t>All indicator go on, Elevator initializes at Floor 2 with doors open and set timer to 10</t>
   </si>
   <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>Request to move up to Floor 3</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>RequestFloor3 Accepted, UptangenFloor 2, 4, Elevator closes doors and moves up to Floor 3</t>
   </si>
   <si>
-    <t>TC003</t>
-  </si>
-  <si>
     <t>Request to move up to Floor 4</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>RequestFloor4 Accepted, UptangenFloor 2, 3, Elevator closes doors and moves up to Floor 4</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>Request to move down to Floor 2</t>
   </si>
   <si>
@@ -85,18 +76,12 @@
     <t>RequestFloor2 Accepted, UptangenFloor 3,4, Elevator closes doors and moves down to Floor 2</t>
   </si>
   <si>
-    <t>TC005</t>
-  </si>
-  <si>
     <t>Request to move down to Floor 3 from Floor 4</t>
   </si>
   <si>
     <t>RequestFloor3 Accepted, UptangenFloor 2,4, Elevator closes doors and moves down to Floor 3</t>
   </si>
   <si>
-    <t>TC006</t>
-  </si>
-  <si>
     <t>Request to open door at Floor 3</t>
   </si>
   <si>
@@ -109,9 +94,6 @@
     <t>DOOR open and timer is reset to 7</t>
   </si>
   <si>
-    <t>TC007</t>
-  </si>
-  <si>
     <t>Ignore door open request while moving</t>
   </si>
   <si>
@@ -121,9 +103,6 @@
     <t>Elevator ignores request</t>
   </si>
   <si>
-    <t>TC008</t>
-  </si>
-  <si>
     <t>Reject request for current floor</t>
   </si>
   <si>
@@ -133,9 +112,6 @@
     <t>Request is the same as req_open_door should open the elevator door</t>
   </si>
   <si>
-    <t>TC009</t>
-  </si>
-  <si>
     <t>Multiple requests queue</t>
   </si>
   <si>
@@ -148,9 +124,6 @@
     <t>Elevator only receive floor 3 request in log, perform transition to floor 3, ignore other</t>
   </si>
   <si>
-    <t>TC010</t>
-  </si>
-  <si>
     <t>Elevator remains idle when no request</t>
   </si>
   <si>
@@ -163,18 +136,12 @@
     <t>Elevator remains at Floor 2 with doors open with timer 10, after 10s, door is closed</t>
   </si>
   <si>
-    <t>TC011</t>
-  </si>
-  <si>
     <t>Request multiple floors while moving</t>
   </si>
   <si>
     <t>Request Floor 4 while going up to Floor 3</t>
   </si>
   <si>
-    <t>TC012</t>
-  </si>
-  <si>
     <t>Request to stop while moving</t>
   </si>
   <si>
@@ -187,9 +154,6 @@
     <t>Not implemented</t>
   </si>
   <si>
-    <t>TC013</t>
-  </si>
-  <si>
     <t>Request lower floor while moving up</t>
   </si>
   <si>
@@ -199,9 +163,6 @@
     <t>Request is ignored, elevator continues to Floor 3</t>
   </si>
   <si>
-    <t>TC014</t>
-  </si>
-  <si>
     <t>Request higher floor while moving down</t>
   </si>
   <si>
@@ -211,9 +172,6 @@
     <t>Request is ignored, elevator continues to Floor 2</t>
   </si>
   <si>
-    <t>TC015</t>
-  </si>
-  <si>
     <t>Call another floor after reaching destination</t>
   </si>
   <si>
@@ -223,9 +181,6 @@
     <t>Elevator moves to Floor 3 after reaching Floor 4</t>
   </si>
   <si>
-    <t>TC016</t>
-  </si>
-  <si>
     <t>Request to open door while door is closing</t>
   </si>
   <si>
@@ -235,9 +190,6 @@
     <t>Request is not ignored, door will pause and reopen with reset time to 7</t>
   </si>
   <si>
-    <t>TC019</t>
-  </si>
-  <si>
     <t>Open Door</t>
   </si>
   <si>
@@ -247,9 +199,6 @@
     <t>Door should open and send out an event DOOR_IS_OPEN if elevator at idle</t>
   </si>
   <si>
-    <t>TC020</t>
-  </si>
-  <si>
     <t>Verify door closes on DOOR_CLOSE command</t>
   </si>
   <si>
@@ -259,9 +208,6 @@
     <t>Door should close</t>
   </si>
   <si>
-    <t>TC021</t>
-  </si>
-  <si>
     <t>Check door opens/closes within expected time</t>
   </si>
   <si>
@@ -274,9 +220,6 @@
     <t>Time taken should be 5s for closing or opening</t>
   </si>
   <si>
-    <t>TC023</t>
-  </si>
-  <si>
     <t>Ensure GO_DOWN command moves elevator down</t>
   </si>
   <si>
@@ -289,9 +232,6 @@
     <t>When controller sends cmd 'GO DOWN', elevator GO down with an event GOdown to Floor 3 or Floor 2</t>
   </si>
   <si>
-    <t>TC024</t>
-  </si>
-  <si>
     <t>Ensure GO_UP command moves elevator up</t>
   </si>
   <si>
@@ -304,63 +244,42 @@
     <t>When controller sends cmd 'GO UP', elevator GO UP with an event GOdown to Floor 3 or Floor 2</t>
   </si>
   <si>
-    <t>TC026</t>
-  </si>
-  <si>
     <t>Ensure initialization on power ON</t>
   </si>
   <si>
     <t>Turn ON power</t>
   </si>
   <si>
-    <t>TC027</t>
-  </si>
-  <si>
     <t>Verify event creation at Floor 2</t>
   </si>
   <si>
     <t>Reach Floor 2</t>
   </si>
   <si>
-    <t>TC028</t>
-  </si>
-  <si>
     <t>Verify event creation at Floor 2.5</t>
   </si>
   <si>
     <t>Reach Floor 2.5</t>
   </si>
   <si>
-    <t>TC029</t>
-  </si>
-  <si>
     <t>Verify event creation at Floor 3</t>
   </si>
   <si>
     <t>Reach Floor 3</t>
   </si>
   <si>
-    <t>TC030</t>
-  </si>
-  <si>
     <t>Verify event creation at Floor 3.5</t>
   </si>
   <si>
     <t>Reach Floor 3.5</t>
   </si>
   <si>
-    <t>TC031</t>
-  </si>
-  <si>
     <t>Verify event creation at Floor 4</t>
   </si>
   <si>
     <t>Reach Floor 4</t>
   </si>
   <si>
-    <t>TC032</t>
-  </si>
-  <si>
     <t>Ignore invalid control combinations</t>
   </si>
   <si>
@@ -370,9 +289,6 @@
     <t>Elevator ignores invalid commands</t>
   </si>
   <si>
-    <t>TC033</t>
-  </si>
-  <si>
     <t>Verify door closes automatically after timerExpired() at Floor 2</t>
   </si>
   <si>
@@ -382,27 +298,18 @@
     <t>Door should close after 7s</t>
   </si>
   <si>
-    <t>TC034</t>
-  </si>
-  <si>
     <t>Verify door closes automatically after timerExpired() at Floor 3</t>
   </si>
   <si>
     <t>Wait for timer to expire at Floor 3</t>
   </si>
   <si>
-    <t>TC035</t>
-  </si>
-  <si>
     <t>Verify door closes automatically after timerExpired() at Floor 4</t>
   </si>
   <si>
     <t>Wait for timer to expire at Floor 4</t>
   </si>
   <si>
-    <t>TC036</t>
-  </si>
-  <si>
     <t>Prevent movement while door is open</t>
   </si>
   <si>
@@ -412,9 +319,6 @@
     <t>Ignore all request (except stop or poweroff) until door is closed</t>
   </si>
   <si>
-    <t>TC037</t>
-  </si>
-  <si>
     <t>Prevent floor request while door is opening</t>
   </si>
   <si>
@@ -424,9 +328,6 @@
     <t>Elevator ignores request until door is closed</t>
   </si>
   <si>
-    <t>TC038</t>
-  </si>
-  <si>
     <t>Verify elevator does not take a new request while processing</t>
   </si>
   <si>
@@ -436,9 +337,6 @@
     <t>Only complete the current request, others are ignored</t>
   </si>
   <si>
-    <t>TC039</t>
-  </si>
-  <si>
     <t>Verify door remains open when requested repeatedly</t>
   </si>
   <si>
@@ -466,10 +364,22 @@
     <t>Door close after 7s</t>
   </si>
   <si>
-    <t>Door remains open or  open while closing and timer reset</t>
-  </si>
-  <si>
     <t>Event generated, log that it reach the floor, indicate idle, opening or closing at that floor, update the floor, elevator pos indicator</t>
+  </si>
+  <si>
+    <t>FSM Transition</t>
+  </si>
+  <si>
+    <t>Door Test</t>
+  </si>
+  <si>
+    <t>Motion Test</t>
+  </si>
+  <si>
+    <t>Sensor Test</t>
+  </si>
+  <si>
+    <t>Door have to fully close then can be open and reset timer, does not pause the door and open while closing</t>
   </si>
 </sst>
 </file>
@@ -968,10 +878,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1350,12 +1262,12 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="96.5703125" bestFit="1" customWidth="1"/>
@@ -1381,7 +1293,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1392,467 +1304,467 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>108</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>146</v>
+        <v>58</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>145</v>
+        <v>61</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>93</v>
+        <v>72</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>143</v>
+        <v>109</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>149</v>
+        <v>110</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>149</v>
+      <c r="E28" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>115</v>
+        <v>88</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,118 +1772,118 @@
         <v>116</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>129</v>
+        <v>98</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>137</v>
+        <v>104</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>148</v>
+      <c r="A36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>